<commit_message>
- Enhanced error handling by ensuring consistent return values in case of exceptions.
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/ApproveRequest.xlsx
+++ b/ProjectTest65/Excel/ApproveRequest.xlsx
@@ -1,81 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C300B320-B44F-4FEE-8454-582002093C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1908" windowWidth="17280" windowHeight="8112" xr2:uid="{31D82B20-6550-4E2E-8D60-2B892439DAA7}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1608" yWindow="3156" windowWidth="17280" windowHeight="8112" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ApproveRequest" sheetId="1" r:id="rId1"/>
+    <sheet name="ApproveRequest" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Execute</t>
-  </si>
-  <si>
-    <t>Test Case</t>
-  </si>
-  <si>
-    <t>Class Converage ID</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Revise</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="Aptos Narrow"/>
+      <charset val="222"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="222"/>
-      <scheme val="minor"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,29 +48,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -425,36 +467,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E21F9E1-BA8F-4F21-B29F-A6A3A3ABE5C8}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.8"/>
   <cols>
-    <col min="3" max="3" width="16.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.296875" bestFit="1" customWidth="1"/>
+    <col width="8.796875" customWidth="1" style="1" min="1" max="2"/>
+    <col width="16.296875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="17.3984375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="16.296875" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="1" s="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Execute</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>TestCase</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Expected</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>ActualResult</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>อนุมัติคำขอ</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ทำการอนุมัติคำขอสำเร็จ</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>no message</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ไม่อนุมัติคำขอ</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ไม่ได้รับการอนุมัตคำขอ</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>no message</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
       </c>
     </row>
+    <row r="4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update report.html with new test suite and statistics for addExpenseTest
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/ApproveRequest.xlsx
+++ b/ProjectTest65/Excel/ApproveRequest.xlsx
@@ -1,43 +1,166 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1922021-00E0-44E4-AE72-1D0A7B13B709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1608" yWindow="3156" windowWidth="17280" windowHeight="8112" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="10695" yWindow="3870" windowWidth="16965" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ApproveRequest" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ApproveRequest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>ActualResult</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Revise</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>อนุมัติคำขอ</t>
+  </si>
+  <si>
+    <t>ทำการอนุมัติคำขอสำเร็จ</t>
+  </si>
+  <si>
+    <t>no message</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>ไม่อนุมัติคำขอ</t>
+  </si>
+  <si>
+    <t>ไม่ได้รับการอนุมัตคำขอ</t>
+  </si>
+  <si>
+    <t>สรุปผลการทดสอบ</t>
+  </si>
+  <si>
+    <t>คิดเป็น %</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <charset val="222"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
+    </font>
+    <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -64,90 +187,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -467,124 +550,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="8.796875" customWidth="1" style="1" min="1" max="2"/>
-    <col width="16.296875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="17.3984375" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="16.296875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col min="1" max="2" width="8.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Execute</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>TestCase</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Condition</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Expected</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>ActualResult</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Result</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="n">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>อนุมัติคำขอ</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>ทำการอนุมัติคำขอสำเร็จ</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>no message</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ไม่อนุมัติคำขอ</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ไม่ได้รับการอนุมัตคำขอ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>no message</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-    </row>
-    <row r="4"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6">
+        <f>COUNTIF(F:F,"Pass")</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="6" t="str">
+        <f>TEXT(J6/2,"0.00%")</f>
+        <v>0.00%</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="7">
+        <f>COUNTIF(F:F,"Fail")</f>
+        <v>2</v>
+      </c>
+      <c r="K7" s="7" t="str">
+        <f>TEXT(J7/2,"0.00%")</f>
+        <v>100.00%</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="6">
+        <f>COUNTIF(G:G,"Pass")</f>
+        <v>2</v>
+      </c>
+      <c r="K12" s="6" t="str">
+        <f>TEXT(J12/2,"0.00%")</f>
+        <v>100.00%</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="7">
+        <f>COUNTIF(G:G,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="7" t="str">
+        <f>TEXT(J13/2,"0.00%")</f>
+        <v>0.00%</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:J11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor code structure and remove redundant sections for improved readability and maintainability
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/ApproveRequest.xlsx
+++ b/ProjectTest65/Excel/ApproveRequest.xlsx
@@ -1,141 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1462C0-2B40-4E3B-AC23-0B4BE46B87B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ApproveRequest" sheetId="1" r:id="rId1"/>
+    <sheet name="ApproveRequest" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
-  <si>
-    <t>Execute</t>
-  </si>
-  <si>
-    <t>TestCase</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Expected</t>
-  </si>
-  <si>
-    <t>ActualResult</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Revise</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>อนุมัติคำขอ</t>
-  </si>
-  <si>
-    <t>ทำการอนุมัติคำขอสำเร็จ</t>
-  </si>
-  <si>
-    <t>no message</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>ไม่อนุมัติคำขอ</t>
-  </si>
-  <si>
-    <t>ไม่ได้รับการอนุมัตคำขอ</t>
-  </si>
-  <si>
-    <t>สรุปผลการทดสอบ</t>
-  </si>
-  <si>
-    <t>คิดเป็น %</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
+      <name val="Aptos Narrow"/>
+      <charset val="222"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="222"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
+      <name val="Aptos Narrow"/>
+      <charset val="222"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="222"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Aptos Narrow"/>
+      <charset val="222"/>
+      <family val="2"/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="222"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Aptos Narrow"/>
+      <charset val="222"/>
+      <family val="2"/>
+      <color rgb="FF9C0006"/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="222"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -152,19 +75,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -194,59 +117,118 @@
     </border>
   </borders>
   <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -566,180 +548,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="2" width="8.69921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col width="8.75" customWidth="1" style="1" min="1" max="2"/>
+    <col width="16.25" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="18.375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="16.25" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row r="1" customFormat="1" s="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Execute</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>TestCase</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>Expected</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>ActualResult</t>
+        </is>
+      </c>
+      <c r="F1" s="9" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>อนุมัติคำขอ</t>
+        </is>
+      </c>
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>ทำการอนุมัติคำขอสำเร็จ</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>no message</t>
+        </is>
+      </c>
+      <c r="F2" s="7" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G2" s="7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="7">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I6" s="3" t="s">
-        <v>17</v>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>ไม่อนุมัติคำขอ</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>ไม่ได้รับการอนุมัตคำขอ</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>no message</t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="I4" s="10" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="I5" s="11" t="inlineStr">
+        <is>
+          <t>สรุปผลการทดสอบ</t>
+        </is>
+      </c>
+      <c r="K5" s="11" t="inlineStr">
+        <is>
+          <t>คิดเป็น %</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
       </c>
       <c r="J6" s="3">
         <f>COUNTIF(F:F,"Pass")</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="3" t="str">
+        <v/>
+      </c>
+      <c r="K6" s="3">
         <f>TEXT(J6/2,"0.00%")</f>
-        <v>0.00%</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I7" s="4" t="s">
-        <v>11</v>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="I7" s="4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
       </c>
       <c r="J7" s="4">
         <f>COUNTIF(F:F,"Fail")</f>
-        <v>2</v>
-      </c>
-      <c r="K7" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K7" s="4">
         <f>TEXT(J7/2,"0.00%")</f>
-        <v>100.00%</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I12" s="3" t="s">
-        <v>17</v>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="I10" s="10" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="I11" s="11" t="inlineStr">
+        <is>
+          <t>สรุปผลการทดสอบ</t>
+        </is>
+      </c>
+      <c r="K11" s="11" t="inlineStr">
+        <is>
+          <t>คิดเป็น %</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
       </c>
       <c r="J12" s="3">
         <f>COUNTIF(G:G,"Pass")</f>
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="str">
+        <v/>
+      </c>
+      <c r="K12" s="3">
         <f>TEXT(J12/2,"0.00%")</f>
-        <v>100.00%</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I13" s="4" t="s">
-        <v>11</v>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="I13" s="4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
       </c>
       <c r="J13" s="4">
         <f>COUNTIF(G:G,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K13" s="4">
         <f>TEXT(J13/2,"0.00%")</f>
-        <v>0.00%</v>
+        <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>